<commit_message>
Created column that totals all of the second set of sampling dates.
</commit_message>
<xml_diff>
--- a/Project_Plan/Analysis_Time_Worksheet_11Feb2019JKB_SD.xlsx
+++ b/Project_Plan/Analysis_Time_Worksheet_11Feb2019JKB_SD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950E40B5-F795-4E17-9055-569DCDC0A8BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F904D3A-978F-4AEC-BB32-42571FB8F18B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2940" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling_Plan" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="80">
   <si>
     <t>Sound Analysis Time</t>
   </si>
@@ -261,6 +261,18 @@
   </si>
   <si>
     <t>18, 19</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Other Option</t>
+  </si>
+  <si>
+    <t>Total number of days of recordings</t>
+  </si>
+  <si>
+    <t>Number of days with divers</t>
   </si>
 </sst>
 </file>
@@ -1239,27 +1251,276 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="49" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="50" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1288,255 +1549,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="49" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="50" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
   </cellXfs>
@@ -1826,10 +1838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F11287C-6B85-44DE-A4AF-43D9C6758D76}">
-  <dimension ref="A1:T74"/>
+  <dimension ref="A1:U74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1849,7 +1861,7 @@
     <col min="14" max="14" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>26</v>
       </c>
@@ -1874,7 +1886,7 @@
       <c r="P1" s="35"/>
       <c r="Q1" s="35"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>28</v>
       </c>
@@ -1896,16 +1908,16 @@
       <c r="P2" s="35"/>
       <c r="Q2" s="35"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="147" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="148"/>
       <c r="F3" s="120"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -1919,24 +1931,26 @@
       <c r="P3" s="35"/>
       <c r="Q3" s="35"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="124" t="s">
         <v>61</v>
       </c>
       <c r="B4" s="125" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="211" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="125" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="178" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="212"/>
-      <c r="F4" s="212"/>
-      <c r="G4" s="212"/>
-      <c r="H4" s="212"/>
-      <c r="I4" s="212"/>
-      <c r="J4" s="212"/>
-      <c r="K4" s="212"/>
+      <c r="E4" s="179"/>
+      <c r="F4" s="179"/>
+      <c r="G4" s="179"/>
+      <c r="H4" s="179"/>
+      <c r="I4" s="179"/>
+      <c r="J4" s="179"/>
+      <c r="K4" s="179"/>
       <c r="L4" s="35"/>
       <c r="M4" s="35"/>
       <c r="N4" s="35"/>
@@ -1944,24 +1958,28 @@
       <c r="P4" s="35"/>
       <c r="Q4" s="35"/>
     </row>
-    <row r="5" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="126" t="s">
-        <v>19</v>
+    <row r="5" spans="1:21" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="128" t="s">
+        <v>63</v>
       </c>
       <c r="B5" s="127">
-        <v>65</v>
-      </c>
-      <c r="C5" s="35"/>
+        <f>COUNT(B24:F31)</f>
+        <v>40</v>
+      </c>
+      <c r="C5" s="127">
+        <f>COUNT(H30:L36)</f>
+        <v>35</v>
+      </c>
       <c r="D5" s="115"/>
       <c r="E5" s="65"/>
       <c r="F5" s="65"/>
       <c r="G5" s="65"/>
-      <c r="H5" s="171" t="s">
+      <c r="H5" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="171"/>
-      <c r="J5" s="171"/>
-      <c r="K5" s="171"/>
+      <c r="I5" s="170"/>
+      <c r="J5" s="170"/>
+      <c r="K5" s="170"/>
       <c r="L5" s="35"/>
       <c r="M5" s="35"/>
       <c r="N5" s="35"/>
@@ -1969,24 +1987,28 @@
       <c r="P5" s="35"/>
       <c r="Q5" s="35"/>
     </row>
-    <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="128" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="B6" s="127">
-        <v>4</v>
-      </c>
-      <c r="C6" s="35"/>
+        <f>COUNT(B34:F38)</f>
+        <v>25</v>
+      </c>
+      <c r="C6" s="127">
+        <f>COUNT(H40:L44)</f>
+        <v>25</v>
+      </c>
       <c r="D6" s="55"/>
       <c r="E6" s="37"/>
       <c r="F6" s="91" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="92"/>
-      <c r="H6" s="173"/>
-      <c r="I6" s="173"/>
-      <c r="J6" s="173"/>
-      <c r="K6" s="173"/>
+      <c r="H6" s="171"/>
+      <c r="I6" s="171"/>
+      <c r="J6" s="171"/>
+      <c r="K6" s="171"/>
       <c r="L6" s="35"/>
       <c r="M6" s="35"/>
       <c r="N6" s="35"/>
@@ -1994,14 +2016,18 @@
       <c r="P6" s="35"/>
       <c r="Q6" s="35"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="128" t="s">
-        <v>63</v>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="126" t="s">
+        <v>78</v>
       </c>
       <c r="B7" s="127">
-        <v>40</v>
-      </c>
-      <c r="C7" s="35"/>
+        <f>COUNT(B24:F31)+ COUNT(B34:F38)</f>
+        <v>65</v>
+      </c>
+      <c r="C7" s="127">
+        <f>COUNT(H30:L36)+ COUNT(H40:L44)</f>
+        <v>60</v>
+      </c>
       <c r="D7" s="116" t="s">
         <v>15</v>
       </c>
@@ -2020,10 +2046,10 @@
       <c r="I7" s="13">
         <v>40</v>
       </c>
-      <c r="J7" s="175" t="s">
+      <c r="J7" s="172" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="239"/>
+      <c r="K7" s="173"/>
       <c r="L7" s="35"/>
       <c r="M7" s="35"/>
       <c r="N7" s="35"/>
@@ -2031,14 +2057,16 @@
       <c r="P7" s="35"/>
       <c r="Q7" s="35"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="128" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="B8" s="127">
-        <v>25</v>
-      </c>
-      <c r="C8" s="35"/>
+        <v>4</v>
+      </c>
+      <c r="C8" s="127">
+        <v>4</v>
+      </c>
       <c r="D8" s="117" t="s">
         <v>17</v>
       </c>
@@ -2057,10 +2085,10 @@
       <c r="I8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="177" t="s">
+      <c r="J8" s="174" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="179"/>
+      <c r="K8" s="175"/>
       <c r="L8" s="35"/>
       <c r="M8" s="35"/>
       <c r="N8" s="35"/>
@@ -2068,15 +2096,18 @@
       <c r="P8" s="35"/>
       <c r="Q8" s="35"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="128" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="127">
-        <f>B5*B6</f>
+        <f>B7*B8</f>
         <v>260</v>
       </c>
-      <c r="C9" s="35"/>
+      <c r="C9" s="127">
+        <f>C7*C8</f>
+        <v>240</v>
+      </c>
       <c r="D9" s="62"/>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -2092,15 +2123,16 @@
       <c r="P9" s="35"/>
       <c r="Q9" s="35"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="128" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="B10" s="127">
-        <f>9*4</f>
-        <v>36</v>
-      </c>
-      <c r="C10" s="35"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="127">
+        <v>12</v>
+      </c>
       <c r="D10" s="38"/>
       <c r="E10" s="8"/>
       <c r="F10" s="93" t="s">
@@ -2118,15 +2150,18 @@
       <c r="P10" s="35"/>
       <c r="Q10" s="35"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="128" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="127">
-        <f t="shared" ref="B11" si="0">B9-B10</f>
-        <v>224</v>
-      </c>
-      <c r="C11" s="35"/>
+        <f>B10*B8</f>
+        <v>36</v>
+      </c>
+      <c r="C11" s="127">
+        <f>C10*C8</f>
+        <v>48</v>
+      </c>
       <c r="D11" s="116" t="s">
         <v>15</v>
       </c>
@@ -2153,16 +2188,30 @@
       <c r="O11" s="35"/>
       <c r="P11" s="35"/>
       <c r="Q11" s="35"/>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S11" s="128" t="s">
+        <v>63</v>
+      </c>
+      <c r="T11" s="127">
+        <f>COUNT(B24:F31)</f>
+        <v>40</v>
+      </c>
+      <c r="U11" s="127">
+        <f>COUNT(H30:L36)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="128" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B12" s="127">
-        <f>B11/40</f>
-        <v>5.6</v>
-      </c>
-      <c r="C12" s="35"/>
+        <f>B9-B11</f>
+        <v>224</v>
+      </c>
+      <c r="C12" s="127">
+        <f>C9-C11</f>
+        <v>192</v>
+      </c>
       <c r="D12" s="118" t="s">
         <v>18</v>
       </c>
@@ -2181,33 +2230,48 @@
       <c r="I12" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="240" t="s">
+      <c r="J12" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="241"/>
+      <c r="K12" s="177"/>
       <c r="L12" s="120"/>
       <c r="M12" s="35"/>
       <c r="N12" s="35"/>
       <c r="O12" s="35"/>
       <c r="P12" s="35"/>
       <c r="Q12" s="35"/>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="46">
-        <v>43181</v>
-      </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="242" t="s">
+      <c r="S12" s="128" t="s">
+        <v>64</v>
+      </c>
+      <c r="T12" s="127">
+        <f>COUNT(B34:F38)</f>
+        <v>25</v>
+      </c>
+      <c r="U12" s="127">
+        <f>COUNT(H40:L44)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="127">
+        <f>B12/40</f>
+        <v>5.6</v>
+      </c>
+      <c r="C13" s="127">
+        <f>C12/40</f>
+        <v>4.8</v>
+      </c>
+      <c r="D13" s="149" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="168"/>
-      <c r="F13" s="168"/>
-      <c r="G13" s="168"/>
-      <c r="H13" s="168"/>
-      <c r="I13" s="243"/>
+      <c r="E13" s="148"/>
+      <c r="F13" s="148"/>
+      <c r="G13" s="148"/>
+      <c r="H13" s="148"/>
+      <c r="I13" s="150"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="35"/>
@@ -2217,18 +2281,24 @@
       <c r="P13" s="35"/>
       <c r="Q13" s="35"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="35"/>
+    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="46">
+        <v>43181</v>
+      </c>
+      <c r="C14" s="46">
+        <v>43182</v>
+      </c>
       <c r="D14" s="109"/>
-      <c r="E14" s="148" t="s">
+      <c r="E14" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="149"/>
-      <c r="G14" s="149"/>
-      <c r="H14" s="149"/>
-      <c r="I14" s="245"/>
+      <c r="F14" s="153"/>
+      <c r="G14" s="153"/>
+      <c r="H14" s="153"/>
+      <c r="I14" s="154"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="L14" s="35"/>
@@ -2238,7 +2308,7 @@
       <c r="P14" s="35"/>
       <c r="Q14" s="35"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="35"/>
@@ -2267,7 +2337,7 @@
       <c r="P15" s="35"/>
       <c r="Q15" s="35"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="35"/>
@@ -2349,43 +2419,43 @@
       <c r="Q18" s="35"/>
     </row>
     <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="195" t="s">
+      <c r="A19" s="198" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="151" t="s">
+      <c r="B19" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="152"/>
-      <c r="D19" s="152"/>
-      <c r="E19" s="152"/>
-      <c r="F19" s="153"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="202"/>
+      <c r="F19" s="203"/>
       <c r="G19" s="132"/>
-      <c r="H19" s="230" t="s">
+      <c r="H19" s="158" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="231"/>
-      <c r="J19" s="231"/>
-      <c r="K19" s="231"/>
-      <c r="L19" s="232"/>
-      <c r="M19" s="229"/>
-      <c r="N19" s="229"/>
-      <c r="O19" s="229"/>
-      <c r="P19" s="229"/>
-      <c r="Q19" s="229"/>
+      <c r="I19" s="159"/>
+      <c r="J19" s="159"/>
+      <c r="K19" s="159"/>
+      <c r="L19" s="160"/>
+      <c r="M19" s="157"/>
+      <c r="N19" s="157"/>
+      <c r="O19" s="157"/>
+      <c r="P19" s="157"/>
+      <c r="Q19" s="157"/>
     </row>
     <row r="20" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="196"/>
+      <c r="A20" s="199"/>
       <c r="B20" s="85"/>
       <c r="C20" s="86"/>
       <c r="D20" s="86"/>
       <c r="E20" s="86"/>
       <c r="F20" s="87"/>
       <c r="G20" s="133"/>
-      <c r="H20" s="233"/>
-      <c r="I20" s="206"/>
-      <c r="J20" s="206"/>
-      <c r="K20" s="206"/>
-      <c r="L20" s="234"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="162"/>
+      <c r="J20" s="162"/>
+      <c r="K20" s="162"/>
+      <c r="L20" s="163"/>
       <c r="M20" s="105"/>
       <c r="N20" s="105"/>
       <c r="O20" s="105"/>
@@ -2393,18 +2463,18 @@
       <c r="Q20" s="105"/>
     </row>
     <row r="21" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="196"/>
+      <c r="A21" s="199"/>
       <c r="B21" s="85"/>
       <c r="C21" s="86"/>
       <c r="D21" s="86"/>
       <c r="E21" s="86"/>
       <c r="F21" s="87"/>
       <c r="G21" s="133"/>
-      <c r="H21" s="233"/>
-      <c r="I21" s="206"/>
-      <c r="J21" s="206"/>
-      <c r="K21" s="206"/>
-      <c r="L21" s="234"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="162"/>
+      <c r="J21" s="162"/>
+      <c r="K21" s="162"/>
+      <c r="L21" s="163"/>
       <c r="M21" s="105"/>
       <c r="N21" s="105"/>
       <c r="O21" s="105"/>
@@ -2412,7 +2482,7 @@
       <c r="Q21" s="105"/>
     </row>
     <row r="22" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="228"/>
+      <c r="A22" s="200"/>
       <c r="B22" s="82" t="s">
         <v>3</v>
       </c>
@@ -2421,11 +2491,11 @@
       <c r="E22" s="83"/>
       <c r="F22" s="84"/>
       <c r="G22" s="133"/>
-      <c r="H22" s="233"/>
-      <c r="I22" s="206"/>
-      <c r="J22" s="206"/>
-      <c r="K22" s="206"/>
-      <c r="L22" s="234"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="162"/>
+      <c r="J22" s="162"/>
+      <c r="K22" s="162"/>
+      <c r="L22" s="163"/>
       <c r="M22" s="120"/>
       <c r="N22" s="120"/>
       <c r="O22" s="120"/>
@@ -2451,14 +2521,14 @@
       <c r="F23" s="12">
         <v>40</v>
       </c>
-      <c r="G23" s="238" t="s">
+      <c r="G23" s="155" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="233"/>
-      <c r="I23" s="206"/>
-      <c r="J23" s="206"/>
-      <c r="K23" s="206"/>
-      <c r="L23" s="234"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="162"/>
+      <c r="J23" s="162"/>
+      <c r="K23" s="162"/>
+      <c r="L23" s="163"/>
       <c r="M23" s="35"/>
       <c r="N23" s="35"/>
       <c r="O23" s="35"/>
@@ -2482,12 +2552,12 @@
       <c r="F24" s="32">
         <v>11</v>
       </c>
-      <c r="G24" s="238"/>
-      <c r="H24" s="235"/>
-      <c r="I24" s="236"/>
-      <c r="J24" s="236"/>
-      <c r="K24" s="236"/>
-      <c r="L24" s="237"/>
+      <c r="G24" s="155"/>
+      <c r="H24" s="164"/>
+      <c r="I24" s="165"/>
+      <c r="J24" s="165"/>
+      <c r="K24" s="165"/>
+      <c r="L24" s="166"/>
       <c r="M24" s="35"/>
       <c r="N24" s="35"/>
       <c r="O24" s="35"/>
@@ -2511,14 +2581,14 @@
       <c r="F25" s="32">
         <v>13</v>
       </c>
-      <c r="G25" s="238"/>
-      <c r="H25" s="213" t="s">
+      <c r="G25" s="155"/>
+      <c r="H25" s="180" t="s">
         <v>70</v>
       </c>
-      <c r="I25" s="198"/>
-      <c r="J25" s="198"/>
-      <c r="K25" s="198"/>
-      <c r="L25" s="214"/>
+      <c r="I25" s="181"/>
+      <c r="J25" s="181"/>
+      <c r="K25" s="181"/>
+      <c r="L25" s="182"/>
       <c r="M25" s="35"/>
       <c r="N25" s="35"/>
       <c r="O25" s="35"/>
@@ -2542,12 +2612,12 @@
       <c r="F26" s="32">
         <v>15</v>
       </c>
-      <c r="G26" s="238"/>
-      <c r="H26" s="215"/>
-      <c r="I26" s="201"/>
-      <c r="J26" s="201"/>
-      <c r="K26" s="201"/>
-      <c r="L26" s="216"/>
+      <c r="G26" s="155"/>
+      <c r="H26" s="183"/>
+      <c r="I26" s="184"/>
+      <c r="J26" s="184"/>
+      <c r="K26" s="184"/>
+      <c r="L26" s="185"/>
       <c r="M26" s="35"/>
       <c r="N26" s="35"/>
       <c r="O26" s="35"/>
@@ -2571,12 +2641,12 @@
       <c r="F27" s="32">
         <v>17</v>
       </c>
-      <c r="G27" s="238"/>
-      <c r="H27" s="217"/>
-      <c r="I27" s="204"/>
-      <c r="J27" s="204"/>
-      <c r="K27" s="204"/>
-      <c r="L27" s="218"/>
+      <c r="G27" s="155"/>
+      <c r="H27" s="186"/>
+      <c r="I27" s="187"/>
+      <c r="J27" s="187"/>
+      <c r="K27" s="187"/>
+      <c r="L27" s="188"/>
       <c r="M27" s="35"/>
       <c r="N27" s="35"/>
       <c r="O27" s="35"/>
@@ -2600,14 +2670,14 @@
       <c r="F28" s="32">
         <v>19</v>
       </c>
-      <c r="G28" s="238"/>
-      <c r="H28" s="208" t="s">
+      <c r="G28" s="155"/>
+      <c r="H28" s="167" t="s">
         <v>67</v>
       </c>
-      <c r="I28" s="209"/>
-      <c r="J28" s="209"/>
-      <c r="K28" s="209"/>
-      <c r="L28" s="210"/>
+      <c r="I28" s="168"/>
+      <c r="J28" s="168"/>
+      <c r="K28" s="168"/>
+      <c r="L28" s="169"/>
       <c r="M28" s="35"/>
       <c r="N28" s="35"/>
       <c r="O28" s="35"/>
@@ -2631,7 +2701,7 @@
       <c r="F29" s="32">
         <v>21</v>
       </c>
-      <c r="G29" s="238"/>
+      <c r="G29" s="155"/>
       <c r="H29" s="135">
         <v>32</v>
       </c>
@@ -2670,7 +2740,7 @@
       <c r="F30" s="32">
         <v>23</v>
       </c>
-      <c r="G30" s="238"/>
+      <c r="G30" s="155"/>
       <c r="H30" s="136">
         <v>12</v>
       </c>
@@ -2709,7 +2779,7 @@
       <c r="F31" s="32">
         <v>25</v>
       </c>
-      <c r="G31" s="238"/>
+      <c r="G31" s="155"/>
       <c r="H31" s="138">
         <v>14</v>
       </c>
@@ -2823,7 +2893,7 @@
       <c r="F34" s="73">
         <v>18</v>
       </c>
-      <c r="G34" s="238" t="s">
+      <c r="G34" s="155" t="s">
         <v>4</v>
       </c>
       <c r="H34" s="136">
@@ -2865,7 +2935,7 @@
       <c r="F35" s="32">
         <v>20</v>
       </c>
-      <c r="G35" s="238"/>
+      <c r="G35" s="155"/>
       <c r="H35" s="136">
         <v>22</v>
       </c>
@@ -2905,7 +2975,7 @@
       <c r="F36" s="97">
         <v>22</v>
       </c>
-      <c r="G36" s="238"/>
+      <c r="G36" s="155"/>
       <c r="H36" s="139">
         <v>24</v>
       </c>
@@ -2945,14 +3015,14 @@
       <c r="F37" s="97">
         <v>24</v>
       </c>
-      <c r="G37" s="238"/>
-      <c r="H37" s="219" t="s">
+      <c r="G37" s="155"/>
+      <c r="H37" s="189" t="s">
         <v>50</v>
       </c>
-      <c r="I37" s="220"/>
-      <c r="J37" s="220"/>
-      <c r="K37" s="220"/>
-      <c r="L37" s="221"/>
+      <c r="I37" s="190"/>
+      <c r="J37" s="190"/>
+      <c r="K37" s="190"/>
+      <c r="L37" s="191"/>
       <c r="M37" s="35"/>
       <c r="N37" s="35"/>
       <c r="O37" s="35"/>
@@ -2977,14 +3047,14 @@
       <c r="F38" s="101">
         <v>26</v>
       </c>
-      <c r="G38" s="246"/>
-      <c r="H38" s="208" t="s">
+      <c r="G38" s="156"/>
+      <c r="H38" s="167" t="s">
         <v>68</v>
       </c>
-      <c r="I38" s="209"/>
-      <c r="J38" s="209"/>
-      <c r="K38" s="209"/>
-      <c r="L38" s="210"/>
+      <c r="I38" s="168"/>
+      <c r="J38" s="168"/>
+      <c r="K38" s="168"/>
+      <c r="L38" s="169"/>
       <c r="M38" s="35"/>
       <c r="N38" s="35"/>
       <c r="O38" s="35"/>
@@ -2994,13 +3064,13 @@
     </row>
     <row r="39" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="112"/>
-      <c r="B39" s="244" t="s">
+      <c r="B39" s="151" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="244"/>
-      <c r="D39" s="244"/>
-      <c r="E39" s="244"/>
-      <c r="F39" s="244"/>
+      <c r="C39" s="151"/>
+      <c r="D39" s="151"/>
+      <c r="E39" s="151"/>
+      <c r="F39" s="151"/>
       <c r="G39" s="108"/>
       <c r="H39" s="135">
         <v>32</v>
@@ -3053,14 +3123,14 @@
       <c r="Q40" s="35"/>
     </row>
     <row r="41" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="225" t="s">
+      <c r="A41" s="195" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="226"/>
-      <c r="C41" s="226"/>
-      <c r="D41" s="226"/>
-      <c r="E41" s="226"/>
-      <c r="F41" s="227"/>
+      <c r="B41" s="196"/>
+      <c r="C41" s="196"/>
+      <c r="D41" s="196"/>
+      <c r="E41" s="196"/>
+      <c r="F41" s="197"/>
       <c r="G41" s="10"/>
       <c r="H41" s="136">
         <v>21</v>
@@ -3085,13 +3155,13 @@
     </row>
     <row r="42" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="109"/>
-      <c r="B42" s="222" t="s">
+      <c r="B42" s="192" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="223"/>
-      <c r="D42" s="223"/>
-      <c r="E42" s="223"/>
-      <c r="F42" s="224"/>
+      <c r="C42" s="193"/>
+      <c r="D42" s="193"/>
+      <c r="E42" s="193"/>
+      <c r="F42" s="194"/>
       <c r="G42" s="10"/>
       <c r="H42" s="136">
         <v>23</v>
@@ -3724,11 +3794,10 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="D13:I13"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="G34:G38"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:F19"/>
     <mergeCell ref="M19:Q19"/>
     <mergeCell ref="H19:L24"/>
     <mergeCell ref="G23:G31"/>
@@ -3737,14 +3806,15 @@
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="J12:K12"/>
+    <mergeCell ref="H25:L27"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="D13:I13"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="G34:G38"/>
     <mergeCell ref="H38:L38"/>
     <mergeCell ref="D4:K4"/>
-    <mergeCell ref="H25:L27"/>
     <mergeCell ref="H37:L37"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3802,104 +3872,104 @@
       <c r="A3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="147" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="168"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="148"/>
+      <c r="F3" s="148"/>
+      <c r="G3" s="148"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="147" t="s">
+      <c r="A4" s="236" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="147"/>
-      <c r="C4" s="147"/>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="147"/>
-      <c r="H4" s="147"/>
-      <c r="I4" s="147"/>
-      <c r="J4" s="147"/>
-      <c r="K4" s="147"/>
-      <c r="L4" s="147"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="147"/>
-      <c r="O4" s="147"/>
-      <c r="P4" s="147"/>
-      <c r="Q4" s="147"/>
-      <c r="R4" s="147"/>
+      <c r="B4" s="236"/>
+      <c r="C4" s="236"/>
+      <c r="D4" s="236"/>
+      <c r="E4" s="236"/>
+      <c r="F4" s="236"/>
+      <c r="G4" s="236"/>
+      <c r="H4" s="236"/>
+      <c r="I4" s="236"/>
+      <c r="J4" s="236"/>
+      <c r="K4" s="236"/>
+      <c r="L4" s="236"/>
+      <c r="M4" s="236"/>
+      <c r="N4" s="236"/>
+      <c r="O4" s="236"/>
+      <c r="P4" s="236"/>
+      <c r="Q4" s="236"/>
+      <c r="R4" s="236"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="147"/>
-      <c r="B5" s="147"/>
-      <c r="C5" s="147"/>
-      <c r="D5" s="147"/>
-      <c r="E5" s="147"/>
-      <c r="F5" s="147"/>
-      <c r="G5" s="147"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="147"/>
-      <c r="L5" s="147"/>
-      <c r="M5" s="147"/>
-      <c r="N5" s="147"/>
-      <c r="O5" s="147"/>
-      <c r="P5" s="147"/>
-      <c r="Q5" s="147"/>
-      <c r="R5" s="147"/>
+      <c r="A5" s="236"/>
+      <c r="B5" s="236"/>
+      <c r="C5" s="236"/>
+      <c r="D5" s="236"/>
+      <c r="E5" s="236"/>
+      <c r="F5" s="236"/>
+      <c r="G5" s="236"/>
+      <c r="H5" s="236"/>
+      <c r="I5" s="236"/>
+      <c r="J5" s="236"/>
+      <c r="K5" s="236"/>
+      <c r="L5" s="236"/>
+      <c r="M5" s="236"/>
+      <c r="N5" s="236"/>
+      <c r="O5" s="236"/>
+      <c r="P5" s="236"/>
+      <c r="Q5" s="236"/>
+      <c r="R5" s="236"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="147"/>
-      <c r="B6" s="147"/>
-      <c r="C6" s="147"/>
-      <c r="D6" s="147"/>
-      <c r="E6" s="147"/>
-      <c r="F6" s="147"/>
-      <c r="G6" s="147"/>
-      <c r="H6" s="147"/>
-      <c r="I6" s="147"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="147"/>
-      <c r="L6" s="147"/>
-      <c r="M6" s="147"/>
-      <c r="N6" s="147"/>
-      <c r="O6" s="147"/>
-      <c r="P6" s="147"/>
-      <c r="Q6" s="147"/>
-      <c r="R6" s="147"/>
+      <c r="A6" s="236"/>
+      <c r="B6" s="236"/>
+      <c r="C6" s="236"/>
+      <c r="D6" s="236"/>
+      <c r="E6" s="236"/>
+      <c r="F6" s="236"/>
+      <c r="G6" s="236"/>
+      <c r="H6" s="236"/>
+      <c r="I6" s="236"/>
+      <c r="J6" s="236"/>
+      <c r="K6" s="236"/>
+      <c r="L6" s="236"/>
+      <c r="M6" s="236"/>
+      <c r="N6" s="236"/>
+      <c r="O6" s="236"/>
+      <c r="P6" s="236"/>
+      <c r="Q6" s="236"/>
+      <c r="R6" s="236"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="147"/>
-      <c r="B7" s="147"/>
-      <c r="C7" s="147"/>
-      <c r="D7" s="147"/>
-      <c r="E7" s="147"/>
-      <c r="F7" s="147"/>
-      <c r="G7" s="147"/>
-      <c r="H7" s="147"/>
-      <c r="I7" s="147"/>
-      <c r="J7" s="147"/>
-      <c r="K7" s="147"/>
-      <c r="L7" s="147"/>
-      <c r="M7" s="147"/>
-      <c r="N7" s="147"/>
-      <c r="O7" s="147"/>
-      <c r="P7" s="147"/>
-      <c r="Q7" s="147"/>
-      <c r="R7" s="147"/>
+      <c r="A7" s="236"/>
+      <c r="B7" s="236"/>
+      <c r="C7" s="236"/>
+      <c r="D7" s="236"/>
+      <c r="E7" s="236"/>
+      <c r="F7" s="236"/>
+      <c r="G7" s="236"/>
+      <c r="H7" s="236"/>
+      <c r="I7" s="236"/>
+      <c r="J7" s="236"/>
+      <c r="K7" s="236"/>
+      <c r="L7" s="236"/>
+      <c r="M7" s="236"/>
+      <c r="N7" s="236"/>
+      <c r="O7" s="236"/>
+      <c r="P7" s="236"/>
+      <c r="Q7" s="236"/>
+      <c r="R7" s="236"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
     </row>
@@ -3921,18 +3991,18 @@
       <c r="G8" s="65"/>
       <c r="H8" s="65"/>
       <c r="I8" s="65"/>
-      <c r="J8" s="171" t="s">
+      <c r="J8" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="171"/>
-      <c r="L8" s="171"/>
-      <c r="M8" s="172"/>
-      <c r="N8" s="157" t="s">
+      <c r="K8" s="170"/>
+      <c r="L8" s="170"/>
+      <c r="M8" s="215"/>
+      <c r="N8" s="240" t="s">
         <v>42</v>
       </c>
-      <c r="O8" s="158"/>
-      <c r="P8" s="158"/>
-      <c r="Q8" s="159"/>
+      <c r="O8" s="241"/>
+      <c r="P8" s="241"/>
+      <c r="Q8" s="242"/>
       <c r="R8" s="66"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -3953,18 +4023,18 @@
       <c r="E9" s="35"/>
       <c r="F9" s="55"/>
       <c r="G9" s="37"/>
-      <c r="H9" s="180" t="s">
+      <c r="H9" s="222" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="180"/>
-      <c r="J9" s="173"/>
-      <c r="K9" s="173"/>
-      <c r="L9" s="173"/>
-      <c r="M9" s="174"/>
-      <c r="N9" s="160"/>
-      <c r="O9" s="161"/>
-      <c r="P9" s="161"/>
-      <c r="Q9" s="162"/>
+      <c r="I9" s="222"/>
+      <c r="J9" s="171"/>
+      <c r="K9" s="171"/>
+      <c r="L9" s="171"/>
+      <c r="M9" s="216"/>
+      <c r="N9" s="243"/>
+      <c r="O9" s="244"/>
+      <c r="P9" s="244"/>
+      <c r="Q9" s="245"/>
       <c r="R9" s="35"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -4001,10 +4071,10 @@
       <c r="K10" s="13">
         <v>40</v>
       </c>
-      <c r="L10" s="175" t="s">
+      <c r="L10" s="172" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="176"/>
+      <c r="M10" s="220"/>
       <c r="N10" s="47" t="s">
         <v>13</v>
       </c>
@@ -4056,10 +4126,10 @@
       <c r="K11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="177" t="s">
+      <c r="L11" s="174" t="s">
         <v>21</v>
       </c>
-      <c r="M11" s="178"/>
+      <c r="M11" s="221"/>
       <c r="N11" s="51">
         <v>2017</v>
       </c>
@@ -4136,10 +4206,10 @@
       <c r="E13" s="10"/>
       <c r="F13" s="38"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="181" t="s">
+      <c r="H13" s="223" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="181"/>
+      <c r="I13" s="223"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="39"/>
@@ -4248,10 +4318,10 @@
       <c r="K15" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="177" t="s">
+      <c r="L15" s="174" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="179"/>
+      <c r="M15" s="175"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
@@ -4291,20 +4361,20 @@
       <c r="D17" s="68"/>
       <c r="E17" s="68"/>
       <c r="F17" s="69"/>
-      <c r="G17" s="206" t="s">
+      <c r="G17" s="162" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="206"/>
-      <c r="I17" s="206"/>
-      <c r="J17" s="206"/>
-      <c r="K17" s="207"/>
-      <c r="L17" s="197" t="s">
+      <c r="H17" s="162"/>
+      <c r="I17" s="162"/>
+      <c r="J17" s="162"/>
+      <c r="K17" s="212"/>
+      <c r="L17" s="205" t="s">
         <v>47</v>
       </c>
-      <c r="M17" s="198"/>
-      <c r="N17" s="198"/>
-      <c r="O17" s="198"/>
-      <c r="P17" s="199"/>
+      <c r="M17" s="181"/>
+      <c r="N17" s="181"/>
+      <c r="O17" s="181"/>
+      <c r="P17" s="206"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
@@ -4327,16 +4397,16 @@
       <c r="F18" s="12">
         <v>40</v>
       </c>
-      <c r="G18" s="206"/>
-      <c r="H18" s="206"/>
-      <c r="I18" s="206"/>
-      <c r="J18" s="206"/>
-      <c r="K18" s="207"/>
-      <c r="L18" s="200"/>
-      <c r="M18" s="201"/>
-      <c r="N18" s="201"/>
-      <c r="O18" s="201"/>
-      <c r="P18" s="202"/>
+      <c r="G18" s="162"/>
+      <c r="H18" s="162"/>
+      <c r="I18" s="162"/>
+      <c r="J18" s="162"/>
+      <c r="K18" s="212"/>
+      <c r="L18" s="207"/>
+      <c r="M18" s="184"/>
+      <c r="N18" s="184"/>
+      <c r="O18" s="184"/>
+      <c r="P18" s="208"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
@@ -4361,16 +4431,16 @@
       <c r="F19" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206"/>
-      <c r="J19" s="206"/>
-      <c r="K19" s="207"/>
-      <c r="L19" s="203"/>
-      <c r="M19" s="204"/>
-      <c r="N19" s="204"/>
-      <c r="O19" s="204"/>
-      <c r="P19" s="205"/>
+      <c r="G19" s="162"/>
+      <c r="H19" s="162"/>
+      <c r="I19" s="162"/>
+      <c r="J19" s="162"/>
+      <c r="K19" s="212"/>
+      <c r="L19" s="209"/>
+      <c r="M19" s="187"/>
+      <c r="N19" s="187"/>
+      <c r="O19" s="187"/>
+      <c r="P19" s="210"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
@@ -4395,18 +4465,18 @@
       <c r="F20" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206"/>
-      <c r="J20" s="206"/>
-      <c r="K20" s="207"/>
-      <c r="L20" s="148" t="s">
+      <c r="G20" s="162"/>
+      <c r="H20" s="162"/>
+      <c r="I20" s="162"/>
+      <c r="J20" s="162"/>
+      <c r="K20" s="212"/>
+      <c r="L20" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="M20" s="149"/>
-      <c r="N20" s="149"/>
-      <c r="O20" s="149"/>
-      <c r="P20" s="150"/>
+      <c r="M20" s="153"/>
+      <c r="N20" s="153"/>
+      <c r="O20" s="153"/>
+      <c r="P20" s="211"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
@@ -4419,11 +4489,11 @@
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
       <c r="F21" s="35"/>
-      <c r="G21" s="206"/>
-      <c r="H21" s="206"/>
-      <c r="I21" s="206"/>
-      <c r="J21" s="206"/>
-      <c r="K21" s="207"/>
+      <c r="G21" s="162"/>
+      <c r="H21" s="162"/>
+      <c r="I21" s="162"/>
+      <c r="J21" s="162"/>
+      <c r="K21" s="212"/>
       <c r="L21" s="17">
         <v>32</v>
       </c>
@@ -4451,11 +4521,11 @@
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
       <c r="F22" s="35"/>
-      <c r="G22" s="206"/>
-      <c r="H22" s="206"/>
-      <c r="I22" s="206"/>
-      <c r="J22" s="206"/>
-      <c r="K22" s="207"/>
+      <c r="G22" s="162"/>
+      <c r="H22" s="162"/>
+      <c r="I22" s="162"/>
+      <c r="J22" s="162"/>
+      <c r="K22" s="212"/>
       <c r="L22" s="31">
         <v>12</v>
       </c>
@@ -4712,13 +4782,13 @@
       <c r="I30" s="35"/>
       <c r="J30" s="35"/>
       <c r="K30" s="35"/>
-      <c r="L30" s="148" t="s">
+      <c r="L30" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="M30" s="149"/>
-      <c r="N30" s="149"/>
-      <c r="O30" s="149"/>
-      <c r="P30" s="150"/>
+      <c r="M30" s="153"/>
+      <c r="N30" s="153"/>
+      <c r="O30" s="153"/>
+      <c r="P30" s="211"/>
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
       <c r="S30" s="10"/>
@@ -4939,74 +5009,74 @@
       <c r="T37" s="10"/>
     </row>
     <row r="38" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="195" t="s">
+      <c r="A38" s="198" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="182" t="s">
+      <c r="B38" s="224" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="183"/>
-      <c r="D38" s="183"/>
-      <c r="E38" s="183"/>
-      <c r="F38" s="184"/>
-      <c r="G38" s="188" t="s">
+      <c r="C38" s="225"/>
+      <c r="D38" s="225"/>
+      <c r="E38" s="225"/>
+      <c r="F38" s="226"/>
+      <c r="G38" s="230" t="s">
         <v>25</v>
       </c>
-      <c r="H38" s="189"/>
-      <c r="I38" s="189"/>
-      <c r="J38" s="189"/>
-      <c r="K38" s="190"/>
-      <c r="L38" s="151" t="s">
+      <c r="H38" s="231"/>
+      <c r="I38" s="231"/>
+      <c r="J38" s="231"/>
+      <c r="K38" s="232"/>
+      <c r="L38" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="M38" s="152"/>
-      <c r="N38" s="152"/>
-      <c r="O38" s="152"/>
-      <c r="P38" s="153"/>
+      <c r="M38" s="202"/>
+      <c r="N38" s="202"/>
+      <c r="O38" s="202"/>
+      <c r="P38" s="203"/>
       <c r="Q38" s="22"/>
       <c r="R38" s="14"/>
       <c r="S38" s="14"/>
       <c r="T38" s="14"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="196"/>
-      <c r="B39" s="185"/>
-      <c r="C39" s="186"/>
-      <c r="D39" s="186"/>
-      <c r="E39" s="186"/>
-      <c r="F39" s="187"/>
-      <c r="G39" s="191"/>
-      <c r="H39" s="192"/>
-      <c r="I39" s="192"/>
-      <c r="J39" s="192"/>
-      <c r="K39" s="193"/>
-      <c r="L39" s="154"/>
-      <c r="M39" s="155"/>
-      <c r="N39" s="155"/>
-      <c r="O39" s="155"/>
-      <c r="P39" s="156"/>
+      <c r="A39" s="199"/>
+      <c r="B39" s="227"/>
+      <c r="C39" s="228"/>
+      <c r="D39" s="228"/>
+      <c r="E39" s="228"/>
+      <c r="F39" s="229"/>
+      <c r="G39" s="233"/>
+      <c r="H39" s="234"/>
+      <c r="I39" s="234"/>
+      <c r="J39" s="234"/>
+      <c r="K39" s="235"/>
+      <c r="L39" s="237"/>
+      <c r="M39" s="238"/>
+      <c r="N39" s="238"/>
+      <c r="O39" s="238"/>
+      <c r="P39" s="239"/>
       <c r="Q39" s="23"/>
       <c r="R39" s="14"/>
       <c r="S39" s="14"/>
       <c r="T39" s="14"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="196"/>
-      <c r="B40" s="185"/>
-      <c r="C40" s="186"/>
-      <c r="D40" s="186"/>
-      <c r="E40" s="186"/>
-      <c r="F40" s="187"/>
-      <c r="G40" s="191"/>
-      <c r="H40" s="192"/>
-      <c r="I40" s="192"/>
-      <c r="J40" s="192"/>
-      <c r="K40" s="193"/>
-      <c r="L40" s="154"/>
-      <c r="M40" s="155"/>
-      <c r="N40" s="155"/>
-      <c r="O40" s="155"/>
-      <c r="P40" s="156"/>
+      <c r="A40" s="199"/>
+      <c r="B40" s="227"/>
+      <c r="C40" s="228"/>
+      <c r="D40" s="228"/>
+      <c r="E40" s="228"/>
+      <c r="F40" s="229"/>
+      <c r="G40" s="233"/>
+      <c r="H40" s="234"/>
+      <c r="I40" s="234"/>
+      <c r="J40" s="234"/>
+      <c r="K40" s="235"/>
+      <c r="L40" s="237"/>
+      <c r="M40" s="238"/>
+      <c r="N40" s="238"/>
+      <c r="O40" s="238"/>
+      <c r="P40" s="239"/>
       <c r="Q40" s="23"/>
       <c r="R40" s="14"/>
       <c r="S40" s="14"/>
@@ -5014,34 +5084,34 @@
     </row>
     <row r="41" spans="1:20" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="56"/>
-      <c r="B41" s="148" t="s">
+      <c r="B41" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="149"/>
-      <c r="D41" s="149"/>
-      <c r="E41" s="149"/>
-      <c r="F41" s="150"/>
-      <c r="G41" s="148" t="s">
+      <c r="C41" s="153"/>
+      <c r="D41" s="153"/>
+      <c r="E41" s="153"/>
+      <c r="F41" s="211"/>
+      <c r="G41" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="H41" s="149"/>
-      <c r="I41" s="149"/>
-      <c r="J41" s="149"/>
-      <c r="K41" s="150"/>
-      <c r="L41" s="148" t="s">
+      <c r="H41" s="153"/>
+      <c r="I41" s="153"/>
+      <c r="J41" s="153"/>
+      <c r="K41" s="211"/>
+      <c r="L41" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="M41" s="149"/>
-      <c r="N41" s="149"/>
-      <c r="O41" s="149"/>
-      <c r="P41" s="150"/>
+      <c r="M41" s="153"/>
+      <c r="N41" s="153"/>
+      <c r="O41" s="153"/>
+      <c r="P41" s="211"/>
       <c r="Q41" s="23"/>
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>
       <c r="T41" s="10"/>
     </row>
     <row r="42" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="164">
+      <c r="A42" s="217">
         <v>42917</v>
       </c>
       <c r="B42" s="17">
@@ -5089,7 +5159,7 @@
       <c r="P42" s="12">
         <v>40</v>
       </c>
-      <c r="Q42" s="163" t="s">
+      <c r="Q42" s="246" t="s">
         <v>4</v>
       </c>
       <c r="R42" s="10"/>
@@ -5097,7 +5167,7 @@
       <c r="T42" s="10"/>
     </row>
     <row r="43" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="165"/>
+      <c r="A43" s="218"/>
       <c r="B43" s="57">
         <v>11</v>
       </c>
@@ -5143,13 +5213,13 @@
       <c r="P43" s="32">
         <v>11</v>
       </c>
-      <c r="Q43" s="163"/>
+      <c r="Q43" s="246"/>
       <c r="R43" s="10"/>
       <c r="S43" s="10"/>
       <c r="T43" s="10"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="165"/>
+      <c r="A44" s="218"/>
       <c r="B44" s="57">
         <v>16</v>
       </c>
@@ -5195,13 +5265,13 @@
       <c r="P44" s="32">
         <v>13</v>
       </c>
-      <c r="Q44" s="163"/>
+      <c r="Q44" s="246"/>
       <c r="R44" s="10"/>
       <c r="S44" s="10"/>
       <c r="T44" s="10"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="165"/>
+      <c r="A45" s="218"/>
       <c r="B45" s="57">
         <v>21</v>
       </c>
@@ -5247,13 +5317,13 @@
       <c r="P45" s="32">
         <v>15</v>
       </c>
-      <c r="Q45" s="163"/>
+      <c r="Q45" s="246"/>
       <c r="R45" s="10"/>
       <c r="S45" s="10"/>
       <c r="T45" s="10"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="165"/>
+      <c r="A46" s="218"/>
       <c r="B46" s="57"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -5289,13 +5359,13 @@
       <c r="P46" s="32">
         <v>17</v>
       </c>
-      <c r="Q46" s="163"/>
+      <c r="Q46" s="246"/>
       <c r="R46" s="10"/>
       <c r="S46" s="10"/>
       <c r="T46" s="10"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="165"/>
+      <c r="A47" s="218"/>
       <c r="B47" s="57"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -5331,13 +5401,13 @@
       <c r="P47" s="32">
         <v>19</v>
       </c>
-      <c r="Q47" s="163"/>
+      <c r="Q47" s="246"/>
       <c r="R47" s="10"/>
       <c r="S47" s="10"/>
       <c r="T47" s="10"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="165"/>
+      <c r="A48" s="218"/>
       <c r="B48" s="57"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -5363,13 +5433,13 @@
       <c r="P48" s="32">
         <v>21</v>
       </c>
-      <c r="Q48" s="163"/>
+      <c r="Q48" s="246"/>
       <c r="R48" s="10"/>
       <c r="S48" s="15"/>
       <c r="T48" s="15"/>
     </row>
     <row r="49" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="165"/>
+      <c r="A49" s="218"/>
       <c r="B49" s="57"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
@@ -5395,13 +5465,13 @@
       <c r="P49" s="32">
         <v>23</v>
       </c>
-      <c r="Q49" s="163"/>
+      <c r="Q49" s="246"/>
       <c r="R49" s="10"/>
       <c r="S49" s="16"/>
       <c r="T49" s="16"/>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="166"/>
+      <c r="A50" s="219"/>
       <c r="B50" s="57"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -5427,43 +5497,43 @@
       <c r="P50" s="32">
         <v>25</v>
       </c>
-      <c r="Q50" s="163"/>
+      <c r="Q50" s="246"/>
       <c r="R50" s="10"/>
       <c r="S50" s="10"/>
       <c r="T50" s="10"/>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A51" s="164">
+      <c r="A51" s="217">
         <v>43252</v>
       </c>
-      <c r="B51" s="148" t="s">
+      <c r="B51" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="149"/>
-      <c r="D51" s="149"/>
-      <c r="E51" s="149"/>
-      <c r="F51" s="150"/>
-      <c r="G51" s="148" t="s">
+      <c r="C51" s="153"/>
+      <c r="D51" s="153"/>
+      <c r="E51" s="153"/>
+      <c r="F51" s="211"/>
+      <c r="G51" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="H51" s="149"/>
-      <c r="I51" s="149"/>
-      <c r="J51" s="149"/>
-      <c r="K51" s="150"/>
-      <c r="L51" s="148" t="s">
+      <c r="H51" s="153"/>
+      <c r="I51" s="153"/>
+      <c r="J51" s="153"/>
+      <c r="K51" s="211"/>
+      <c r="L51" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="M51" s="149"/>
-      <c r="N51" s="149"/>
-      <c r="O51" s="149"/>
-      <c r="P51" s="150"/>
+      <c r="M51" s="153"/>
+      <c r="N51" s="153"/>
+      <c r="O51" s="153"/>
+      <c r="P51" s="211"/>
       <c r="Q51" s="58"/>
       <c r="R51" s="10"/>
       <c r="S51" s="10"/>
       <c r="T51" s="10"/>
     </row>
     <row r="52" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="165"/>
+      <c r="A52" s="218"/>
       <c r="B52" s="18">
         <v>32</v>
       </c>
@@ -5515,7 +5585,7 @@
       <c r="T52" s="10"/>
     </row>
     <row r="53" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="165"/>
+      <c r="A53" s="218"/>
       <c r="B53" s="4">
         <v>18</v>
       </c>
@@ -5561,7 +5631,7 @@
       <c r="P53" s="73">
         <v>18</v>
       </c>
-      <c r="Q53" s="169" t="s">
+      <c r="Q53" s="213" t="s">
         <v>4</v>
       </c>
       <c r="R53" s="21"/>
@@ -5569,7 +5639,7 @@
       <c r="T53" s="10"/>
     </row>
     <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="165"/>
+      <c r="A54" s="218"/>
       <c r="B54" s="4">
         <v>23</v>
       </c>
@@ -5615,13 +5685,13 @@
       <c r="P54" s="32">
         <v>20</v>
       </c>
-      <c r="Q54" s="169"/>
+      <c r="Q54" s="213"/>
       <c r="R54" s="10"/>
       <c r="S54" s="10"/>
       <c r="T54" s="10"/>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A55" s="165"/>
+      <c r="A55" s="218"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -5657,13 +5727,13 @@
       <c r="P55" s="32">
         <v>22</v>
       </c>
-      <c r="Q55" s="169"/>
+      <c r="Q55" s="213"/>
       <c r="R55" s="10"/>
       <c r="S55" s="10"/>
       <c r="T55" s="10"/>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A56" s="165"/>
+      <c r="A56" s="218"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -5699,13 +5769,13 @@
       <c r="P56" s="32">
         <v>24</v>
       </c>
-      <c r="Q56" s="169"/>
+      <c r="Q56" s="213"/>
       <c r="R56" s="10"/>
       <c r="S56" s="10"/>
       <c r="T56" s="10"/>
     </row>
     <row r="57" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="166"/>
+      <c r="A57" s="219"/>
       <c r="B57" s="19"/>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
@@ -5731,7 +5801,7 @@
       <c r="P57" s="34">
         <v>26</v>
       </c>
-      <c r="Q57" s="170"/>
+      <c r="Q57" s="214"/>
       <c r="R57" s="10"/>
       <c r="S57" s="10"/>
       <c r="T57" s="10"/>
@@ -5748,13 +5818,13 @@
       <c r="I58" s="10"/>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
-      <c r="L58" s="194" t="s">
+      <c r="L58" s="204" t="s">
         <v>41</v>
       </c>
-      <c r="M58" s="194"/>
-      <c r="N58" s="194"/>
-      <c r="O58" s="194"/>
-      <c r="P58" s="194"/>
+      <c r="M58" s="204"/>
+      <c r="N58" s="204"/>
+      <c r="O58" s="204"/>
+      <c r="P58" s="204"/>
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
       <c r="S58" s="10"/>
@@ -6488,12 +6558,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="L58:P58"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="L17:P19"/>
-    <mergeCell ref="L20:P20"/>
-    <mergeCell ref="L30:P30"/>
-    <mergeCell ref="G17:K22"/>
+    <mergeCell ref="A4:R7"/>
+    <mergeCell ref="L41:P41"/>
+    <mergeCell ref="L38:P40"/>
+    <mergeCell ref="N8:Q9"/>
+    <mergeCell ref="Q42:Q50"/>
+    <mergeCell ref="A42:A50"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="Q53:Q57"/>
     <mergeCell ref="J8:M9"/>
@@ -6510,12 +6580,12 @@
     <mergeCell ref="B38:F40"/>
     <mergeCell ref="G38:K40"/>
     <mergeCell ref="G51:K51"/>
-    <mergeCell ref="A4:R7"/>
-    <mergeCell ref="L41:P41"/>
-    <mergeCell ref="L38:P40"/>
-    <mergeCell ref="N8:Q9"/>
-    <mergeCell ref="Q42:Q50"/>
-    <mergeCell ref="A42:A50"/>
+    <mergeCell ref="L58:P58"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="L17:P19"/>
+    <mergeCell ref="L20:P20"/>
+    <mergeCell ref="L30:P30"/>
+    <mergeCell ref="G17:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>